<commit_message>
updated from day 9 to 20
</commit_message>
<xml_diff>
--- a/Day 2/Day 2 Demo.xlsx
+++ b/Day 2/Day 2 Demo.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rithw\Desktop\Data Analytics\Day 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9E233E3-41A4-474E-8974-1116B8593A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A020C2-394C-4806-85FD-4F1C683E660F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0230BBCB-F22D-4952-AA7D-0434E548D88A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0230BBCB-F22D-4952-AA7D-0434E548D88A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
   <si>
     <t>Date &amp; Time Functions</t>
   </si>
@@ -230,13 +231,43 @@
   </si>
   <si>
     <t>Saturday</t>
+  </si>
+  <si>
+    <t>MONTH</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>CALENDER</t>
+  </si>
+  <si>
+    <t>SUNDAY</t>
+  </si>
+  <si>
+    <t>MONDAY</t>
+  </si>
+  <si>
+    <t>TUESDAY</t>
+  </si>
+  <si>
+    <t>WEDNESDAY</t>
+  </si>
+  <si>
+    <t>THURSDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRIDAY </t>
+  </si>
+  <si>
+    <t>SATURDAY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,8 +289,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,8 +317,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -504,15 +549,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,15 +619,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -574,6 +644,52 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,11 +709,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$A$3" max="12" min="1" page="10" val="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$A$3" max="12" min="1" page="10" val="7"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$C$4" max="9999" min="1000" page="10" val="2020"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$C$4" max="9999" min="1000" page="10" val="2021"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$A$4" max="12" min="1" page="10" val="7"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$A$6" max="3000" min="1900" page="10" val="2021"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -609,13 +733,13 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>15240</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>10160</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>220980</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>193040</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -657,15 +781,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>15242</xdr:colOff>
+          <xdr:colOff>15240</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>10932</xdr:rowOff>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>222307</xdr:colOff>
+          <xdr:colOff>220980</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>194475</xdr:rowOff>
+          <xdr:rowOff>198120</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -675,7 +799,112 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF2BA061-D5D7-4EA8-B7B6-EFEF75F84D86}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>83820</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>586740</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>350520</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2050" name="Spinner 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2050"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>99060</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>358140</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2051" name="Spinner 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2051"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8D41BF8-01F5-4D22-8925-DF3A8DA92256}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1004,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62002F3A-CBC4-447C-925D-E6B0A1EC6165}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1017,13 +1246,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -1037,17 +1266,17 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <f ca="1">TODAY()</f>
-        <v>44385</v>
-      </c>
-      <c r="C3" s="3">
+        <v>44388</v>
+      </c>
+      <c r="C3" s="2">
         <v>44385</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1055,17 +1284,17 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <f ca="1">NOW()</f>
-        <v>44385.356818749999</v>
-      </c>
-      <c r="C4" s="6">
+        <v>44388.68106145833</v>
+      </c>
+      <c r="C4" s="5">
         <v>0.31666666666666665</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1075,9 +1304,9 @@
       </c>
       <c r="B6">
         <f ca="1">HOUR(NOW())</f>
-        <v>8</v>
-      </c>
-      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1087,9 +1316,9 @@
       </c>
       <c r="B7">
         <f ca="1">MINUTE(B4)</f>
-        <v>33</v>
-      </c>
-      <c r="F7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1099,9 +1328,9 @@
       </c>
       <c r="B8">
         <f ca="1">SECOND(B4)</f>
-        <v>49</v>
-      </c>
-      <c r="F8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1109,11 +1338,11 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <f ca="1">TIME(B6,B7,B8)</f>
-        <v>0.35681712962962964</v>
-      </c>
-      <c r="F9" s="4" t="s">
+        <v>0.68106481481481485</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1123,9 +1352,9 @@
       </c>
       <c r="B11">
         <f ca="1">DAY(B3)</f>
-        <v>8</v>
-      </c>
-      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1141,7 +1370,7 @@
         <f ca="1">IFERROR(CHOOSE(B12,"January","February","March","April","May","June","July","August","September","October","November","December"),"Only 1 to 12 is allowed")</f>
         <v>July</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1153,7 +1382,7 @@
         <f ca="1">YEAR(NOW())</f>
         <v>2021</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1161,11 +1390,11 @@
       <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <f ca="1">DATE(B13,B12,B11)</f>
-        <v>44385</v>
-      </c>
-      <c r="F14" s="4" t="s">
+        <v>44388</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1175,9 +1404,9 @@
       </c>
       <c r="B16">
         <f ca="1">WEEKDAY(B14,2)</f>
-        <v>4</v>
-      </c>
-      <c r="F16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1189,7 +1418,7 @@
         <f ca="1">WEEKNUM(B14,2)</f>
         <v>28</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1197,11 +1426,11 @@
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <f ca="1">EOMONTH(B14,0)</f>
         <v>44408</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1209,7 +1438,7 @@
       <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1217,7 +1446,7 @@
       <c r="A21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>34801</v>
       </c>
     </row>
@@ -1225,9 +1454,9 @@
       <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <f ca="1">TODAY()</f>
-        <v>44385</v>
+        <v>44388</v>
       </c>
       <c r="F22" t="s">
         <v>32</v>
@@ -1277,7 +1506,7 @@
       </c>
       <c r="B26">
         <f ca="1">DATEDIF(B21,B22,"d")</f>
-        <v>9584</v>
+        <v>9587</v>
       </c>
       <c r="F26" t="s">
         <v>36</v>
@@ -1307,7 +1536,7 @@
       </c>
       <c r="B28">
         <f ca="1">DATEDIF(B21,B22,"md")</f>
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F28" t="s">
         <v>38</v>
@@ -1322,7 +1551,7 @@
       </c>
       <c r="B29">
         <f ca="1">DATEDIF(B21,B22,"yd")</f>
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1331,9 +1560,9 @@
       </c>
       <c r="B31">
         <f ca="1">DAYS360(B21,B22)</f>
-        <v>9446</v>
-      </c>
-      <c r="F31" s="4" t="s">
+        <v>9449</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1341,7 +1570,7 @@
       <c r="A33" t="s">
         <v>49</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>44150</v>
       </c>
       <c r="D33" t="s">
@@ -1360,7 +1589,7 @@
       <c r="D35" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="3" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1368,7 +1597,7 @@
       <c r="A36" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>44154</v>
       </c>
       <c r="F36" t="s">
@@ -1379,11 +1608,11 @@
       <c r="A37" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <f>WORKDAY(B33,B34,D36:D42)</f>
         <v>44368</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>44165</v>
       </c>
     </row>
@@ -1391,19 +1620,19 @@
       <c r="A38" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <f>WORKDAY.INTL(B33,B34,11,D36:D42)</f>
         <v>44331</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>44190</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>44197</v>
       </c>
     </row>
@@ -1411,18 +1640,18 @@
       <c r="A40" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>44377</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>44222</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>44283</v>
       </c>
       <c r="F41" t="s">
@@ -1433,7 +1662,7 @@
       <c r="A42" t="s">
         <v>56</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>44284</v>
       </c>
     </row>
@@ -1445,7 +1674,7 @@
         <f>NETWORKDAYS(B33,B40,D36:D42)</f>
         <v>157</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1459,7 +1688,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D45" s="8"/>
+      <c r="D45" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1473,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBBEB02-10BE-45B5-8DD9-280BD20A6093}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1486,238 +1715,238 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E2" s="15" t="str">
+      <c r="E2" s="25" t="str">
         <f>"Calendar of "&amp;C3&amp;" "&amp;C4</f>
-        <v>Calendar of October 2020</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="17"/>
+        <v>Calendar of July 2021</v>
+      </c>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="27"/>
     </row>
     <row r="3" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>10</v>
-      </c>
-      <c r="B3" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="25" t="str">
+      <c r="C3" s="21" t="str">
         <f>CHOOSE(A3,"January","February","March","April","May","June","July","August","September","October","November","December")</f>
-        <v>October</v>
-      </c>
-      <c r="E3" s="18" t="s">
+        <v>July</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="27">
-        <v>2020</v>
-      </c>
-      <c r="E4" s="21" t="str">
+      <c r="C4" s="23">
+        <v>2021</v>
+      </c>
+      <c r="E4" s="17" t="str">
         <f>IF(WEEKDAY(DATE($C$4,$A$3,1))=1,1,"")</f>
         <v/>
       </c>
-      <c r="F4" s="12" t="str">
+      <c r="F4" s="11" t="str">
         <f>IFERROR(IF(WEEKDAY(DATE($C$4,$A$3,1))=2,1,E4+1),"")</f>
         <v/>
       </c>
-      <c r="G4" s="12" t="str">
+      <c r="G4" s="11" t="str">
         <f>IFERROR(IF(WEEKDAY(DATE($C$4,$A$3,1))=3,1,F4+1),"")</f>
         <v/>
       </c>
-      <c r="H4" s="12" t="str">
+      <c r="H4" s="11" t="str">
         <f>IFERROR(IF(WEEKDAY(DATE($C$4,$A$3,1))=4,1,G4+1),"")</f>
         <v/>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <f>IFERROR(IF(WEEKDAY(DATE($C$4,$A$3,1))=5,1,H4+1),"")</f>
         <v>1</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="11">
         <f>IFERROR(IF(WEEKDAY(DATE($C$4,$A$3,1))=6,1,I4+1),"")</f>
         <v>2</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="8">
         <f>IFERROR(IF(WEEKDAY(DATE($C$4,$A$3,1))=7,1,J4+1),"")</f>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E5" s="22">
+      <c r="E5" s="18">
         <f>K4+1</f>
         <v>4</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f>E5+1</f>
         <v>5</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <f t="shared" ref="G5:K5" si="0">F5+1</f>
         <v>6</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E6" s="22">
+      <c r="E6" s="18">
         <f t="shared" ref="E6:E7" si="1">K5+1</f>
         <v>11</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f t="shared" ref="F6:K6" si="2">E6+1</f>
         <v>12</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="10">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="12">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E7" s="22">
+      <c r="E7" s="18">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="F7" s="11">
-        <f t="shared" ref="F7:K8" si="3">E7+1</f>
+      <c r="F7" s="10">
+        <f t="shared" ref="F7:K7" si="3">E7+1</f>
         <v>19</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="10">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="12">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E8" s="22">
+      <c r="E8" s="18">
         <f>IFERROR(IF(DAY(EOMONTH(DATE($C$4,$A$3,1),0))=K7,"",K7+1),"")</f>
         <v>25</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f>IFERROR(IF(DAY(EOMONTH(DATE($C$4,$A$3,1),0))=E8,"",E8+1),"")</f>
         <v>26</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <f t="shared" ref="G8:K9" si="4">IFERROR(IF(DAY(EOMONTH(DATE($C$4,$A$3,1),0))=F8,"",F8+1),"")</f>
         <v>27</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="12">
         <f t="shared" si="4"/>
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E9" s="23" t="str">
+      <c r="E9" s="19" t="str">
         <f>IFERROR(IF(DAY(EOMONTH(DATE($C$4,$A$3,1),0))=K8,"",K8+1),"")</f>
         <v/>
       </c>
-      <c r="F9" s="14" t="str">
+      <c r="F9" s="13" t="str">
         <f>IFERROR(IF(DAY(EOMONTH(DATE($C$4,$A$3,1),0))=E9,"",E9+1),"")</f>
         <v/>
       </c>
-      <c r="G9" s="14" t="str">
+      <c r="G9" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="H9" s="14" t="str">
+      <c r="H9" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="I9" s="14" t="str">
+      <c r="I9" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="J9" s="14" t="str">
+      <c r="J9" s="13" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="K9" s="10" t="str">
+      <c r="K9" s="9" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C10" s="8"/>
+      <c r="C10" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1779,4 +2008,220 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E151C7E4-6E2D-4A93-ACB7-8AB79C3AE019}">
+  <dimension ref="A2:M12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.796875" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="7" max="7" width="10.19921875" style="28" customWidth="1"/>
+    <col min="8" max="8" width="11.296875" style="28" customWidth="1"/>
+    <col min="9" max="9" width="10.69921875" style="28" customWidth="1"/>
+    <col min="10" max="10" width="11" style="28" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="28" customWidth="1"/>
+    <col min="12" max="12" width="10.09765625" style="28" customWidth="1"/>
+    <col min="13" max="13" width="12.09765625" style="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G2" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="31"/>
+    </row>
+    <row r="4" spans="1:13" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="30" t="str">
+        <f>CHOOSE(A4,"January","February","March","April","May","June","July","August","September","October","November","December")</f>
+        <v>July</v>
+      </c>
+      <c r="G4" s="35" t="str">
+        <f xml:space="preserve"> "CALENDER OF "&amp; C4&amp;" "&amp;C6</f>
+        <v>CALENDER OF July 2021</v>
+      </c>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="37"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+    </row>
+    <row r="6" spans="1:13" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2021</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="30">
+        <f>A6</f>
+        <v>2021</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G9" s="33"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G10" s="33"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G11" s="33"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G12" s="33"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="G4:M4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2050" r:id="rId4" name="Spinner 2">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>83820</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>586740</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>350520</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2051" r:id="rId5" name="Spinner 3">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>99060</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>571500</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>358140</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
 </file>
</xml_diff>